<commit_message>
change auth request token
</commit_message>
<xml_diff>
--- a/assets/remake.xlsx
+++ b/assets/remake.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korbold/Documents/Kruger/Favorita/Script Filiales/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E64FA5-6718-8F4F-BD9A-F8FEE7343481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11630F5B-4438-154B-89BF-4AF46492DFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68800" yWindow="11500" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68800" yWindow="11520" windowWidth="34560" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulario" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -135,113 +135,107 @@
     <t>RAZON SOCIAL DE FILIAL</t>
   </si>
   <si>
-    <t>0920172483</t>
-  </si>
-  <si>
-    <t>GRACE</t>
-  </si>
-  <si>
-    <t>PATRICIA</t>
-  </si>
-  <si>
-    <t>GONZALEZ</t>
-  </si>
-  <si>
-    <t>PENAFIEL</t>
-  </si>
-  <si>
-    <t>19/06/2025</t>
-  </si>
-  <si>
-    <t>08:14:14 AM</t>
-  </si>
-  <si>
     <t>Cuenta en Legal</t>
   </si>
   <si>
     <t xml:space="preserve">SUKASA/TODOHOGAR </t>
   </si>
   <si>
-    <t>1102956503</t>
-  </si>
-  <si>
-    <t>BETTY</t>
-  </si>
-  <si>
-    <t>YOLANDA</t>
-  </si>
-  <si>
-    <t>JARAMILLO</t>
-  </si>
-  <si>
-    <t>CASTILLO</t>
-  </si>
-  <si>
-    <t>08:07:22 AM</t>
-  </si>
-  <si>
-    <t>0106522055</t>
-  </si>
-  <si>
-    <t>JUAN</t>
-  </si>
-  <si>
-    <t>ESTEBAN</t>
-  </si>
-  <si>
-    <t>COBOS</t>
-  </si>
-  <si>
-    <t>GUEVARA</t>
-  </si>
-  <si>
-    <t>08:04:08 AM</t>
-  </si>
-  <si>
-    <t>0920553005</t>
-  </si>
-  <si>
-    <t>MARIA</t>
-  </si>
-  <si>
-    <t>FERNANDA</t>
-  </si>
-  <si>
-    <t>OBREGON</t>
-  </si>
-  <si>
-    <t>BOLANOS</t>
-  </si>
-  <si>
     <t>18/06/2025</t>
   </si>
   <si>
-    <t>04:22:16 PM</t>
-  </si>
-  <si>
-    <t>0909816928</t>
-  </si>
-  <si>
-    <t>SUSANA</t>
-  </si>
-  <si>
-    <t>MARCELA</t>
-  </si>
-  <si>
-    <t>PAEZ</t>
-  </si>
-  <si>
-    <t>JORQUERA</t>
-  </si>
-  <si>
-    <t>04:21:46 PM</t>
+    <t>0900187576</t>
+  </si>
+  <si>
+    <t>ANA</t>
+  </si>
+  <si>
+    <t>LUCIA</t>
+  </si>
+  <si>
+    <t>JURADO</t>
+  </si>
+  <si>
+    <t>RODAS</t>
+  </si>
+  <si>
+    <t>04:20:56 PM</t>
+  </si>
+  <si>
+    <t>0911976819</t>
+  </si>
+  <si>
+    <t>SORAYA</t>
+  </si>
+  <si>
+    <t>COLOMA</t>
+  </si>
+  <si>
+    <t>MOLINA</t>
+  </si>
+  <si>
+    <t>04:20:33 PM</t>
+  </si>
+  <si>
+    <t>0920355393</t>
+  </si>
+  <si>
+    <t>RAUL</t>
+  </si>
+  <si>
+    <t>MEDARDO</t>
+  </si>
+  <si>
+    <t>SANCHEZ</t>
+  </si>
+  <si>
+    <t>PANCHANA</t>
+  </si>
+  <si>
+    <t>04:19:36 PM</t>
+  </si>
+  <si>
+    <t>0804494003</t>
+  </si>
+  <si>
+    <t>LEONELA</t>
+  </si>
+  <si>
+    <t>JULEISY</t>
+  </si>
+  <si>
+    <t>PULIA</t>
+  </si>
+  <si>
+    <t>ARIAS</t>
+  </si>
+  <si>
+    <t>04:19:11 PM</t>
+  </si>
+  <si>
+    <t>1726612243</t>
+  </si>
+  <si>
+    <t>ESTEFANY</t>
+  </si>
+  <si>
+    <t>AURA</t>
+  </si>
+  <si>
+    <t>CASTRO</t>
+  </si>
+  <si>
+    <t>QUINONES</t>
+  </si>
+  <si>
+    <t>04:18:19 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -266,13 +260,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,17 +335,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +565,7 @@
   <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -666,49 +651,49 @@
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="7">
+        <v>17054</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="7">
-        <v>28964</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="12">
-        <v>1790746119001</v>
-      </c>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="11">
+        <v>1790746119006</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -716,7 +701,7 @@
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -728,37 +713,35 @@
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="7">
+        <v>24787</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="7">
-        <v>25566</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="L3" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="12">
-        <v>1790746119001</v>
-      </c>
-      <c r="P3" s="11" t="s">
+      <c r="O3" s="11">
+        <v>1790746119007</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -766,49 +749,49 @@
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="7">
+        <v>30018</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="7">
-        <v>34660</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="L4" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="12">
-        <v>1790746119001</v>
-      </c>
-      <c r="P4" s="11" t="s">
+      <c r="O4" s="11">
+        <v>1790746119008</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -816,49 +799,49 @@
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="7">
+        <v>34555</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="7">
-        <v>30010</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="12">
-        <v>1790746119001</v>
-      </c>
-      <c r="P5" s="11" t="s">
+      <c r="O5" s="11">
+        <v>1790746119009</v>
+      </c>
+      <c r="P5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -866,49 +849,49 @@
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="I6" s="7">
+        <v>34952</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="7">
-        <v>22662</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>39</v>
+      <c r="L6" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="12">
-        <v>1790746119001</v>
-      </c>
-      <c r="P6" s="11" t="s">
+      <c r="O6" s="11">
+        <v>1790746119010</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -926,24 +909,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>Listas!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
-          <x14:formula1>
-            <xm:f>Listas!$E$2:$E$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>